<commit_message>
updated safenet results and added fmea
</commit_message>
<xml_diff>
--- a/results/safenet_topics_May-04-2022/hazard_interpretation.xlsx
+++ b/results/safenet_topics_May-04-2022/hazard_interpretation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\results\safenet_topics_May-04-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E69488B-253C-452D-AE10-E47B10FA05FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8774971-E25E-48C5-8487-DC5E78E6C22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4944" yWindow="2652" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
+    <workbookView xWindow="14832" yWindow="3432" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard-focused" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="116">
   <si>
     <t>Hazard level 1 topics</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Chainsaw fuel leak</t>
   </si>
   <si>
-    <t>fuel leak</t>
-  </si>
-  <si>
     <t>Food Supply Issues</t>
   </si>
   <si>
@@ -97,12 +94,6 @@
     <t>burn from ground falling underneath</t>
   </si>
   <si>
-    <t xml:space="preserve">degree, burn, second degree burn, </t>
-  </si>
-  <si>
-    <t>heat, exhaustion, heat exhaustion</t>
-  </si>
-  <si>
     <t>Medical</t>
   </si>
   <si>
@@ -151,12 +142,6 @@
     <t>Bandwidth</t>
   </si>
   <si>
-    <t>Radio and Communication Issues</t>
-  </si>
-  <si>
-    <t>heart attack, cardiologist, angioplasty</t>
-  </si>
-  <si>
     <t>10, 29</t>
   </si>
   <si>
@@ -178,112 +163,226 @@
     <t>Heart Attack</t>
   </si>
   <si>
-    <t xml:space="preserve">air, frequency, air ground, channel, air ground frequency, </t>
-  </si>
-  <si>
     <t>Air to Ground Communication</t>
   </si>
   <si>
-    <t>8, 39</t>
+    <t>Inadequate Training or Certification</t>
+  </si>
+  <si>
+    <t>Vehicle Breakdown</t>
+  </si>
+  <si>
+    <t>sleep deprivation, deprivation, fatigue, slept, sleepy, early morning, asleep</t>
+  </si>
+  <si>
+    <t>Fatigue</t>
+  </si>
+  <si>
+    <t>Drug use</t>
+  </si>
+  <si>
+    <t>Cargo operations overhead</t>
+  </si>
+  <si>
+    <t>Poison Oak</t>
+  </si>
+  <si>
+    <t>Insect Stings</t>
+  </si>
+  <si>
+    <t>Some of these are talking about allergic or severe reactions as well as subpar treatment, do we want to include all rashes?</t>
+  </si>
+  <si>
+    <t>Computer network restarts, updates, and outwages affect operations and training</t>
+  </si>
+  <si>
+    <t>qualification, refresher, training, hire, certification, work capacity, unqualified, certificate, untrained, inadequately, falsification, trainee</t>
+  </si>
+  <si>
+    <t>Contamination of water for mission activities, including drops</t>
+  </si>
+  <si>
+    <t>wastewater, bacteria, particulate, contamination, residue, sewage</t>
+  </si>
+  <si>
+    <t>Hazard Subcategory</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>Human Factors</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Red Flag Warning</t>
+  </si>
+  <si>
+    <t>Communications</t>
+  </si>
+  <si>
+    <t>Fuel Leak</t>
+  </si>
+  <si>
+    <t>Insufficient Breaks</t>
+  </si>
+  <si>
+    <t>13, 39</t>
+  </si>
+  <si>
+    <t>13, 23, 41, 30, 35</t>
+  </si>
+  <si>
+    <t>bee, sting, insect, insects, wasp</t>
+  </si>
+  <si>
+    <t>Communication Disruption</t>
+  </si>
+  <si>
+    <t>26, 8</t>
+  </si>
+  <si>
+    <t>25, 40, 5</t>
+  </si>
+  <si>
+    <t>47, 13, 16, 1</t>
+  </si>
+  <si>
+    <t>49, 41, 43</t>
+  </si>
+  <si>
+    <t>Falling Objects</t>
+  </si>
+  <si>
+    <t>Trees during trimming operations, rocks</t>
+  </si>
+  <si>
+    <t>Entrapment</t>
+  </si>
+  <si>
+    <t>2, 43, 35</t>
+  </si>
+  <si>
+    <t>May need to break up into vehicle damage, operator issues, and accidents</t>
+  </si>
+  <si>
+    <t>8, 39, 13</t>
+  </si>
+  <si>
+    <t>heat, heat exhaustion, rhabdomyolysis, stroke</t>
+  </si>
+  <si>
+    <t>heart attack, cardiologist, angioplasty, angina</t>
+  </si>
+  <si>
+    <t>degree, burn, second degree burn</t>
+  </si>
+  <si>
+    <t>air, frequency, air ground, channel, air ground frequency</t>
+  </si>
+  <si>
+    <t>change to reckless or dangerous driving?</t>
+  </si>
+  <si>
+    <t>trap, entrapment, overrun</t>
+  </si>
+  <si>
+    <t>potential</t>
+  </si>
+  <si>
+    <t>mph, speed, speed limit, excessive speed, fast</t>
+  </si>
+  <si>
+    <t>Reckless Driving</t>
+  </si>
+  <si>
+    <t>fuel, fuel cap, drip, leak, spill, spray, gasoline, leakage</t>
+  </si>
+  <si>
+    <t>type, unburned, litter, scba, flare, bottle</t>
+  </si>
+  <si>
+    <t>28, 45, 44, 35, 38, 16, 24, 4</t>
+  </si>
+  <si>
+    <t>pool, exposure</t>
+  </si>
+  <si>
+    <t>drug, illegal, drug use, alcohol, cocaine, marijuana, abuse, intoxicate</t>
+  </si>
+  <si>
+    <t>39, 47, 23, 5, 26, 8, 25, 12, 14, 24, 26, 47</t>
+  </si>
+  <si>
+    <t>tree fell, faller, cut tree, struck, loose, rock, log, hit, debris, weaken tree, snag</t>
+  </si>
+  <si>
+    <t>7, 39</t>
+  </si>
+  <si>
+    <t>red flag, warning, red flag warning</t>
   </si>
   <si>
     <t>16, 39</t>
   </si>
   <si>
-    <t>7, 39</t>
-  </si>
-  <si>
-    <t>food, drink, eat, breakfast, lunch, meal, dinner, calorie, hungry, rotten, rotton</t>
-  </si>
-  <si>
-    <t>bee, sting, insect, insects</t>
-  </si>
-  <si>
-    <t>covid, health, social distance, toxic, sick, exposure, pandemic, expose, test, contract, virus, symptom, infect, illness, nausea, ill, stomach, flu, vomit, hantavirus, pathogen, bronchitis, headache</t>
-  </si>
-  <si>
-    <t>Vehicle Accident</t>
-  </si>
-  <si>
-    <t>vehicle, truck, tire, driver, passenger,inspection, drive, brake, wheel, operator, road, driver side, roll, hit, stuck, stop, accident, caught, crack, slip, broken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">work rest, rest, work rest guideline, awareness, violate, work rest ratio, break, shift, exceed hour, cdl duty day, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">filter, exhaust, regenerate, idle, regen, loss power, power, truck, type engine, regeneration process, exhaust filter, engine, towed, shutdown, </t>
-  </si>
-  <si>
-    <t>Insufficienct Breaks</t>
-  </si>
-  <si>
-    <t>Inadequate Training or Certification</t>
-  </si>
-  <si>
-    <t>Vehicle Breakdown</t>
-  </si>
-  <si>
-    <t>bucket, water drop, bucket drop, load, dip, cargo</t>
-  </si>
-  <si>
-    <t>red flag, flag, red, warning, forecase, red flag warning, high wind</t>
-  </si>
-  <si>
-    <t>sleep deprivation, deprivation, fatigue, slept, sleepy, early morning, asleep</t>
-  </si>
-  <si>
-    <t>drug, illegal, drug use, alcohol, cocaine</t>
-  </si>
-  <si>
-    <t>mph, speed, highway, vehicle, limit, speed limit, excessive speed, fast</t>
-  </si>
-  <si>
-    <t>Speeding</t>
-  </si>
-  <si>
-    <t>Fatigue</t>
-  </si>
-  <si>
-    <t>Drug use</t>
-  </si>
-  <si>
-    <t>Red Flag warming</t>
-  </si>
-  <si>
-    <t>Cargo operations overhead</t>
-  </si>
-  <si>
-    <t>Poison Oak</t>
-  </si>
-  <si>
-    <t>Insect Stings</t>
-  </si>
-  <si>
-    <t>Some of these are talking about allergic or severe reactions as well as subpar treatment, do we want to include all rashes?</t>
-  </si>
-  <si>
-    <t>Computer network restarts, updates, and outwages affect operations and training</t>
-  </si>
-  <si>
-    <t>39, 47</t>
-  </si>
-  <si>
-    <t>25, 40</t>
-  </si>
-  <si>
-    <t>qualification, refresher, training, hire, certification, work capacity, unqualified, certificate, untrained, inadequately, falsification, trainee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fuel, cap, gas, drip, leak, spill, spray, gasoline, </t>
-  </si>
-  <si>
-    <t>Contamination of water for mission activities, including drops</t>
-  </si>
-  <si>
-    <t>wastewater, bacteria, particulate, contamination, residue, sewage</t>
-  </si>
-  <si>
-    <t>28, 45, 44</t>
+    <t>0, 48, 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work rest, rest, work rest guideline, violate, work rest ratio, break, shift, exceed hour, cdl duty day, </t>
+  </si>
+  <si>
+    <t>food, eat, breakfast, lunch, meal, dinner, calorie, hungry, rotten, rotton</t>
+  </si>
+  <si>
+    <t>bucket, water drop, bucket drop, dip, retardant drop, retardant</t>
+  </si>
+  <si>
+    <t>covid, health, social distance, toxic, sick, exposure, pandemic, expose, virus, symptom, infect, illness, nausea, ill, stomach, flu, vomit, hantavirus, pathogen, bronchitis, headache, hepatitis</t>
+  </si>
+  <si>
+    <t>atv</t>
+  </si>
+  <si>
+    <t>Vehicle Collision or Accident</t>
+  </si>
+  <si>
+    <t>Vehicle Damage</t>
+  </si>
+  <si>
+    <t>accident</t>
+  </si>
+  <si>
+    <t>tire, inspection, brake, wheel, driver side, crack, broken, damage, repair, bolt, lug</t>
+  </si>
+  <si>
+    <t>hit, stuck, accident, slip, impact, injury, slid</t>
+  </si>
+  <si>
+    <t>43, 49, 41</t>
+  </si>
+  <si>
+    <t>filter, exhaust, regenerate, idle, regen, loss power, power, type engine, regeneration process, exhaust filter, towed, shutdown, malfunction</t>
+  </si>
+  <si>
+    <t>fatalities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lots of variance here; </t>
+  </si>
+  <si>
+    <t>LOS as backup, cell as back up too</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>injuries</t>
+  </si>
+  <si>
+    <t>damages</t>
   </si>
 </sst>
 </file>
@@ -307,12 +406,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -327,9 +438,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,15 +808,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E799D7D2-7755-4A40-8FAC-FBB6E32500C5}">
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -734,325 +848,738 @@
       <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="1"/>
+      <c r="Q1" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="R1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
-      </c>
-      <c r="R2" t="s">
-        <v>15</v>
+        <v>87</v>
+      </c>
+      <c r="N2" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="T2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R3" t="s">
+        <v>99</v>
+      </c>
+      <c r="P3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" t="s">
         <v>16</v>
       </c>
-      <c r="T3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="P4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" t="s">
+        <v>24</v>
+      </c>
+      <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" t="s">
+        <v>57</v>
+      </c>
+      <c r="R7" t="s">
         <v>22</v>
       </c>
-      <c r="R4" t="s">
-        <v>18</v>
-      </c>
-      <c r="T4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P5" t="s">
-        <v>22</v>
-      </c>
-      <c r="R5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="R7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="P8" t="s">
+        <v>58</v>
       </c>
       <c r="R8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>64</v>
       </c>
       <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" t="s">
+        <v>59</v>
+      </c>
+      <c r="R9" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9" t="s">
+        <v>51</v>
+      </c>
+      <c r="U9">
+        <v>2</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="P10" t="s">
+        <v>59</v>
+      </c>
+      <c r="R10" t="s">
+        <v>50</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+      <c r="P11" t="s">
+        <v>58</v>
+      </c>
+      <c r="R11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R9" t="s">
-        <v>72</v>
-      </c>
-      <c r="T9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>53</v>
-      </c>
-      <c r="R10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="R11" t="s">
-        <v>31</v>
-      </c>
       <c r="T11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="U11">
+        <v>2</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
-      </c>
-      <c r="R12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="P12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="U12">
+        <v>2</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="R13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="P13" t="s">
+        <v>61</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="P14" t="s">
+        <v>61</v>
       </c>
       <c r="R14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
-      </c>
-      <c r="R15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="P15" t="s">
+        <v>58</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
-      </c>
-      <c r="R16" t="s">
-        <v>45</v>
+        <v>55</v>
+      </c>
+      <c r="P16" t="s">
+        <v>58</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="T16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="U16">
+        <v>2</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="P17" t="s">
+        <v>61</v>
       </c>
       <c r="R17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="T17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>81</v>
+      </c>
+      <c r="P18" t="s">
+        <v>61</v>
       </c>
       <c r="R18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>53</v>
+      </c>
+      <c r="P19" t="s">
+        <v>58</v>
       </c>
       <c r="R19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="R20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="U20">
+        <v>2</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>106</v>
+      </c>
+      <c r="N21" t="s">
+        <v>105</v>
+      </c>
+      <c r="P21" t="s">
+        <v>57</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="T21" t="s">
+        <v>76</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>42</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
+        <v>98</v>
+      </c>
+      <c r="P22" t="s">
+        <v>58</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="U22">
+        <v>2</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+      <c r="P23" t="s">
         <v>57</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="U23">
+        <v>2</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>100</v>
+      </c>
+      <c r="P24" t="s">
+        <v>61</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="U24">
+        <v>2</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>95</v>
+      </c>
+      <c r="P25" t="s">
+        <v>61</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" t="s">
+        <v>91</v>
+      </c>
+      <c r="N26" t="s">
+        <v>90</v>
+      </c>
+      <c r="P26" t="s">
+        <v>58</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="P27" t="s">
+        <v>58</v>
+      </c>
+      <c r="R27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="U27">
+        <v>2</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+      <c r="P28" t="s">
+        <v>57</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="T28" t="s">
+        <v>82</v>
+      </c>
+      <c r="U28">
+        <v>1</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" t="s">
+        <v>93</v>
+      </c>
+      <c r="N29" t="s">
+        <v>102</v>
+      </c>
+      <c r="P29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>43</v>
-      </c>
-      <c r="E22" t="s">
-        <v>58</v>
-      </c>
-      <c r="R22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>44</v>
-      </c>
-      <c r="E23" t="s">
-        <v>62</v>
-      </c>
-      <c r="R23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>45</v>
-      </c>
-      <c r="E24" t="s">
-        <v>63</v>
-      </c>
-      <c r="R24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25" t="s">
-        <v>65</v>
-      </c>
-      <c r="R25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>47</v>
-      </c>
-      <c r="E26" t="s">
-        <v>64</v>
-      </c>
-      <c r="R26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>49</v>
-      </c>
-      <c r="E27" t="s">
-        <v>66</v>
-      </c>
-      <c r="R27" t="s">
-        <v>67</v>
+      <c r="R29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="T29" t="s">
+        <v>73</v>
+      </c>
+      <c r="U29">
+        <v>2</v>
+      </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" t="s">
+        <v>83</v>
+      </c>
+      <c r="N30" t="s">
+        <v>84</v>
+      </c>
+      <c r="P30" t="s">
+        <v>59</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="U30">
+        <v>2</v>
+      </c>
+      <c r="V30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>